<commit_message>
add new enum values for reaction monitoring
</commit_message>
<xml_diff>
--- a/docs/cems/cems-metadata.xlsx
+++ b/docs/cems/cems-metadata.xlsx
@@ -342,7 +342,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Mode of data collection in tandem MS assays. Either DDA (Data-dependent acquisition) or DIA (Data-independent acquisition).</t>
+          <t>Mode of data collection in tandem MS assays. Either DDA (Data-dependent acquisition), DIA (Data-independent acquisition), MRM (multiple reaction monitoring), or PRM (parallel reaction monitoring).</t>
         </r>
       </text>
     </comment>
@@ -624,7 +624,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
   <si>
     <t>version</t>
   </si>
@@ -759,6 +759,12 @@
   </si>
   <si>
     <t>DIA</t>
+  </si>
+  <si>
+    <t>MRM</t>
+  </si>
+  <si>
+    <t>PRM</t>
   </si>
   <si>
     <t>ms_scan_mode</t>
@@ -1301,67 +1307,67 @@
         <v>42</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1406,8 +1412,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: TIMS / TWIMS / FAIMS / DTIMS / SLIMS." sqref="W2:W1048576">
       <formula1>'ion_mobility list'!$A$1:$A$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: DDA / DIA." sqref="X2:X1048576">
-      <formula1>'data_collection_mode list'!$A$1:$A$2</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: DDA / DIA / MRM / PRM." sqref="X2:X1048576">
+      <formula1>'data_collection_mode list'!$A$1:$A$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: MS / MS/MS / MS3." sqref="Y2:Y1048576">
       <formula1>'ms_scan_mode list'!$A$1:$A$3</formula1>
@@ -1454,17 +1460,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1482,12 +1488,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1505,17 +1511,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1533,22 +1539,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1566,12 +1572,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1589,12 +1595,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1612,12 +1618,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1813,7 +1819,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1829,6 +1835,16 @@
         <v>44</v>
       </c>
     </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Mccalluc/new data collection modes (#1103)
* Add constraints for consistency

* use include

* Regen - now constrained

* add new enum values for reaction monitoring

* changelog

* more regen
</commit_message>
<xml_diff>
--- a/docs/cems/cems-metadata.xlsx
+++ b/docs/cems/cems-metadata.xlsx
@@ -342,7 +342,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Mode of data collection in tandem MS assays. Either DDA (Data-dependent acquisition) or DIA (Data-independent acquisition).</t>
+          <t>Mode of data collection in tandem MS assays. Either DDA (Data-dependent acquisition), DIA (Data-independent acquisition), MRM (multiple reaction monitoring), or PRM (parallel reaction monitoring).</t>
         </r>
       </text>
     </comment>
@@ -624,7 +624,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
   <si>
     <t>version</t>
   </si>
@@ -759,6 +759,12 @@
   </si>
   <si>
     <t>DIA</t>
+  </si>
+  <si>
+    <t>MRM</t>
+  </si>
+  <si>
+    <t>PRM</t>
   </si>
   <si>
     <t>ms_scan_mode</t>
@@ -1301,67 +1307,67 @@
         <v>42</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1406,8 +1412,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: TIMS / TWIMS / FAIMS / DTIMS / SLIMS." sqref="W2:W1048576">
       <formula1>'ion_mobility list'!$A$1:$A$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: DDA / DIA." sqref="X2:X1048576">
-      <formula1>'data_collection_mode list'!$A$1:$A$2</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: DDA / DIA / MRM / PRM." sqref="X2:X1048576">
+      <formula1>'data_collection_mode list'!$A$1:$A$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: MS / MS/MS / MS3." sqref="Y2:Y1048576">
       <formula1>'ms_scan_mode list'!$A$1:$A$3</formula1>
@@ -1454,17 +1460,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1482,12 +1488,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1505,17 +1511,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1533,22 +1539,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1566,12 +1572,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1589,12 +1595,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1612,12 +1618,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1813,7 +1819,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1829,6 +1835,16 @@
         <v>44</v>
       </c>
     </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>